<commit_message>
added functionality to add sample files and run problems again in new folders
</commit_message>
<xml_diff>
--- a/data/improvement strategies/Classeur2.xlsx
+++ b/data/improvement strategies/Classeur2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fhans/Documents/GenerativeBenchmarking/clone-anonymous-github/ChatGPT-Study-2757/data/improvement strategies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{463F8A47-3818-6C4A-B0F3-9E3F21ADDD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E200371B-A396-204F-9812-C54F5D048B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{00034E20-DE0C-9547-BC2A-B79E68AC1734}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="1" xr2:uid="{00034E20-DE0C-9547-BC2A-B79E68AC1734}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="ideas" sheetId="1" r:id="rId1"/>
+    <sheet name="issue log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Improvement strategies</t>
   </si>
@@ -48,6 +49,80 @@
   </si>
   <si>
     <t>Solve again from scratch (brute force)</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>chatGPT did not follow the provided structure for some problems. It seems that it sometimes deviates from the structure and hallucinates extra long answers with multiple classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ✘ Runtime Error
+  ✘ Error: Line 73: NameError: name 'LFUCache' is not defined
+  ✘ Error: NameError: name 'LFUCache' is not defined
+    obj = LFUCache(__Deserializer__()._deserialize(json.dumps(cargs[0], escape_forward_slashes=False), "integer"))
+Line 73 in _driver (Solution.py)
+    _driver()
+Line 88 in &lt;module&gt; (Solution.py)
+  ✘ Your Input: ["LFUCache","put","put","get","put","get","get","put","get","get","get"]
+[[2],[1,1],[2,2],[1],[3,3],[2],[3],[4,4],[1],[3],[4]]
+  ✘ Expected Answer: 
+  ✘ Stdout: </t>
+  </si>
+  <si>
+    <t>cases passed</t>
+  </si>
+  <si>
+    <t>**stdout:**
+b'  \xe2\x9c\x98 Runtime Error\n  \xe2\x9c\x98 4/16 cases passed (N/A)\n  \xe2\x9c\x98 Error: Line 14: IndexError: list index out of range\n  \xe2\x9c\x98 Error: IndexError: list index out of range\n    stack = self.stacks[stack_index]\nLine 14 in push (Solution.py)\n    result = obj.push(\nLine 45 in __helper_select_method__ (Solution.py)\n    ret.append(__DriverSolution__().__helper_select_method__(method, params[index], obj))\nLine 96 in _driver (Solution.py)\n    _driver()\nLine 105 in &lt;module&gt; (Solution.py)\n  \xe2\x9c\x98 Testcase: ["DinnerPlates","push","push","popAtStack","pop","push","push","pop","pop"]\n\' +\n  \'[[1],[1],[2],[1],[],[1],[2],[],[]]\n  \xe2\x9c\x98 Answer: \n  \xe2\x9c\x98 Expected Answer: [null,null,null,2,1,null,null,2,1]\n  \xe2\x9c\x98 Stdout: \n'</t>
+  </si>
+  <si>
+    <t>ChatGPT does not pass all tests</t>
+  </si>
+  <si>
+    <t>4/16'</t>
+  </si>
+  <si>
+    <t>Try to at least reduce the runtime error (not passing test cases is one thing, not keeping the provided format is another) Maybe even measure the degree runtime errors could be reduced by e.g. saying -&gt; stay true to format or something</t>
+  </si>
+  <si>
+    <t>Try to log each failed test case so it's not like training for triathlon. Passing the one makes you weaker in the other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ✘ Finished
+  ✘ Your Input: ["DinnerPlates","push","push","push","push","push","popAtStack","push","push","popAtStack","popAtStack","pop","pop","pop","pop","pop"]
+[[2],[1],[2],[3],[4],[5],[0],[20],[21],[0],[2],[],[],[],[],[]]
+  ✘ Output (66 ms): [null,null,null,null,null,null,2,null,null,1,20,21,5,4,3,-1]
+  ✘ Expected Answer: [null,null,null,null,null,null,2,null,null,20,21,5,4,3,1,-1]
+  ✘ Stdout: 2
+1
+20
+21
+5
+4
+3
+-1</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
+  <si>
+    <t>error - submit</t>
+  </si>
+  <si>
+    <t>error - test</t>
+  </si>
+  <si>
+    <t>Maybe sometimes the gpt needs to be reminded that it needs to only define functions. To my knowledge the questions never ask to print something to the console</t>
   </si>
 </sst>
 </file>
@@ -90,9 +165,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928F949E-9253-CB42-BF74-397A3B15E418}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" customWidth="1"/>
+    <col min="1" max="1" width="114.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.3">
@@ -438,6 +531,106 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA601F51-43CC-B249-AE5F-CC9983D05EC0}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="113.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="72.5" style="6" customWidth="1"/>
+    <col min="7" max="7" width="70" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>460</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="301" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1172</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>